<commit_message>
added micro front ends
</commit_message>
<xml_diff>
--- a/React.js Curriculum.xlsx
+++ b/React.js Curriculum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\anil\training\react\react_curriculum_latest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B39EA-688C-419C-B684-77739CDAF3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD22231-C084-48A8-A581-B4A523DB2A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{654EB569-EDC2-4BB1-B840-3B6BF14D88E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{654EB569-EDC2-4BB1-B840-3B6BF14D88E8}"/>
   </bookViews>
   <sheets>
     <sheet name="React.js Curriculum" sheetId="1" r:id="rId1"/>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB51E14D-F238-47A7-819B-0424257A8063}">
   <dimension ref="B1:H194"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3102,7 +3102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BFAEFC-F782-4C0E-8D94-36458D0FC464}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>

</xml_diff>